<commit_message>
updates to outliers; initial prophet fit
</commit_message>
<xml_diff>
--- a/Experimental Notebooks/Data/Clean_McBroken_Daily.xlsx
+++ b/Experimental Notebooks/Data/Clean_McBroken_Daily.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1576"/>
+  <dimension ref="A1:G1577"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25655,7 +25655,7 @@
         <v>556250</v>
       </c>
       <c r="F1140" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1140" t="b">
         <v>1</v>
@@ -26092,7 +26092,7 @@
         <v>1637500</v>
       </c>
       <c r="F1159" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1159" t="b">
         <v>1</v>
@@ -31374,7 +31374,7 @@
         <v>1325000</v>
       </c>
       <c r="F1389" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1389" t="b">
         <v>1</v>
@@ -31397,7 +31397,7 @@
         <v>1244375</v>
       </c>
       <c r="F1390" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1390" t="b">
         <v>1</v>
@@ -31420,7 +31420,7 @@
         <v>1255000</v>
       </c>
       <c r="F1391" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1391" t="b">
         <v>1</v>
@@ -31443,7 +31443,7 @@
         <v>1215625</v>
       </c>
       <c r="F1392" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1392" t="b">
         <v>1</v>
@@ -31466,7 +31466,7 @@
         <v>1260625</v>
       </c>
       <c r="F1393" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1393" t="b">
         <v>1</v>
@@ -31489,7 +31489,7 @@
         <v>1340625</v>
       </c>
       <c r="F1394" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1394" t="b">
         <v>1</v>
@@ -31512,7 +31512,7 @@
         <v>1566250</v>
       </c>
       <c r="F1395" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1395" t="b">
         <v>1</v>
@@ -31535,7 +31535,7 @@
         <v>1580625</v>
       </c>
       <c r="F1396" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1396" t="b">
         <v>1</v>
@@ -31558,7 +31558,7 @@
         <v>1578125</v>
       </c>
       <c r="F1397" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1397" t="b">
         <v>1</v>
@@ -31581,7 +31581,7 @@
         <v>1493125</v>
       </c>
       <c r="F1398" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1398" t="b">
         <v>1</v>
@@ -31604,7 +31604,7 @@
         <v>1588750</v>
       </c>
       <c r="F1399" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1399" t="b">
         <v>1</v>
@@ -31627,7 +31627,7 @@
         <v>1637500</v>
       </c>
       <c r="F1400" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1400" t="b">
         <v>1</v>
@@ -31650,7 +31650,7 @@
         <v>1736250</v>
       </c>
       <c r="F1401" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1401" t="b">
         <v>1</v>
@@ -31673,7 +31673,7 @@
         <v>1875625</v>
       </c>
       <c r="F1402" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1402" t="b">
         <v>1</v>
@@ -31696,7 +31696,7 @@
         <v>2058750</v>
       </c>
       <c r="F1403" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1403" t="b">
         <v>1</v>
@@ -31719,7 +31719,7 @@
         <v>2050000</v>
       </c>
       <c r="F1404" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1404" t="b">
         <v>1</v>
@@ -31742,7 +31742,7 @@
         <v>1962500</v>
       </c>
       <c r="F1405" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1405" t="b">
         <v>1</v>
@@ -31765,7 +31765,7 @@
         <v>1658125</v>
       </c>
       <c r="F1406" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1406" t="b">
         <v>1</v>
@@ -31788,7 +31788,7 @@
         <v>1435000</v>
       </c>
       <c r="F1407" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1407" t="b">
         <v>1</v>
@@ -31811,7 +31811,7 @@
         <v>1353125</v>
       </c>
       <c r="F1408" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1408" t="b">
         <v>1</v>
@@ -31834,7 +31834,7 @@
         <v>1520000</v>
       </c>
       <c r="F1409" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1409" t="b">
         <v>1</v>
@@ -31857,7 +31857,7 @@
         <v>1593750</v>
       </c>
       <c r="F1410" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1410" t="b">
         <v>1</v>
@@ -31880,7 +31880,7 @@
         <v>1549375</v>
       </c>
       <c r="F1411" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1411" t="b">
         <v>1</v>
@@ -31903,7 +31903,7 @@
         <v>1383750</v>
       </c>
       <c r="F1412" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1412" t="b">
         <v>1</v>
@@ -31926,7 +31926,7 @@
         <v>1344375</v>
       </c>
       <c r="F1413" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1413" t="b">
         <v>1</v>
@@ -31949,7 +31949,7 @@
         <v>1240625</v>
       </c>
       <c r="F1414" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1414" t="b">
         <v>1</v>
@@ -31972,7 +31972,7 @@
         <v>1183750</v>
       </c>
       <c r="F1415" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1415" t="b">
         <v>1</v>
@@ -31995,7 +31995,7 @@
         <v>1354375</v>
       </c>
       <c r="F1416" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1416" t="b">
         <v>1</v>
@@ -32018,7 +32018,7 @@
         <v>1330000</v>
       </c>
       <c r="F1417" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1417" t="b">
         <v>1</v>
@@ -34995,7 +34995,7 @@
         <v>0</v>
       </c>
       <c r="G1547" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1548">
@@ -35662,6 +35662,29 @@
         <v>0</v>
       </c>
       <c r="G1576" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1577">
+      <c r="A1577" s="2" t="n">
+        <v>45704</v>
+      </c>
+      <c r="B1577" t="n">
+        <v>1283</v>
+      </c>
+      <c r="C1577" t="n">
+        <v>11867</v>
+      </c>
+      <c r="D1577" t="n">
+        <v>10.81149405915564</v>
+      </c>
+      <c r="E1577" t="n">
+        <v>801875</v>
+      </c>
+      <c r="F1577" t="b">
+        <v>0</v>
+      </c>
+      <c r="G1577" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update test load from new setup
</commit_message>
<xml_diff>
--- a/Experimental Notebooks/Data/Clean_McBroken_Daily.xlsx
+++ b/Experimental Notebooks/Data/Clean_McBroken_Daily.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1577"/>
+  <dimension ref="A1:G1583"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35018,7 +35018,7 @@
         <v>0</v>
       </c>
       <c r="G1548" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1549">
@@ -35041,7 +35041,7 @@
         <v>0</v>
       </c>
       <c r="G1549" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1550">
@@ -35064,7 +35064,7 @@
         <v>0</v>
       </c>
       <c r="G1550" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1551">
@@ -35087,7 +35087,7 @@
         <v>0</v>
       </c>
       <c r="G1551" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1552">
@@ -35110,7 +35110,7 @@
         <v>0</v>
       </c>
       <c r="G1552" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1553">
@@ -35133,7 +35133,7 @@
         <v>0</v>
       </c>
       <c r="G1553" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1554">
@@ -35685,6 +35685,144 @@
         <v>0</v>
       </c>
       <c r="G1577" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1578">
+      <c r="A1578" s="2" t="n">
+        <v>45705</v>
+      </c>
+      <c r="B1578" t="n">
+        <v>1364</v>
+      </c>
+      <c r="C1578" t="n">
+        <v>11570</v>
+      </c>
+      <c r="D1578" t="n">
+        <v>11.78910976663786</v>
+      </c>
+      <c r="E1578" t="n">
+        <v>852500</v>
+      </c>
+      <c r="F1578" t="b">
+        <v>0</v>
+      </c>
+      <c r="G1578" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1579">
+      <c r="A1579" s="2" t="n">
+        <v>45706</v>
+      </c>
+      <c r="B1579" t="n">
+        <v>1359</v>
+      </c>
+      <c r="C1579" t="n">
+        <v>11832</v>
+      </c>
+      <c r="D1579" t="n">
+        <v>11.48580121703854</v>
+      </c>
+      <c r="E1579" t="n">
+        <v>849375</v>
+      </c>
+      <c r="F1579" t="b">
+        <v>0</v>
+      </c>
+      <c r="G1579" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1580">
+      <c r="A1580" s="2" t="n">
+        <v>45707</v>
+      </c>
+      <c r="B1580" t="n">
+        <v>1190</v>
+      </c>
+      <c r="C1580" t="n">
+        <v>11835</v>
+      </c>
+      <c r="D1580" t="n">
+        <v>10.05492184199409</v>
+      </c>
+      <c r="E1580" t="n">
+        <v>743750</v>
+      </c>
+      <c r="F1580" t="b">
+        <v>0</v>
+      </c>
+      <c r="G1580" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1581">
+      <c r="A1581" s="2" t="n">
+        <v>45708</v>
+      </c>
+      <c r="B1581" t="n">
+        <v>1207</v>
+      </c>
+      <c r="C1581" t="n">
+        <v>11990</v>
+      </c>
+      <c r="D1581" t="n">
+        <v>10.06672226855713</v>
+      </c>
+      <c r="E1581" t="n">
+        <v>754375</v>
+      </c>
+      <c r="F1581" t="b">
+        <v>0</v>
+      </c>
+      <c r="G1581" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1582">
+      <c r="A1582" s="2" t="n">
+        <v>45709</v>
+      </c>
+      <c r="B1582" t="n">
+        <v>1110</v>
+      </c>
+      <c r="C1582" t="n">
+        <v>11907</v>
+      </c>
+      <c r="D1582" t="n">
+        <v>9.322247417485514</v>
+      </c>
+      <c r="E1582" t="n">
+        <v>693750</v>
+      </c>
+      <c r="F1582" t="b">
+        <v>0</v>
+      </c>
+      <c r="G1582" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1583">
+      <c r="A1583" s="2" t="n">
+        <v>45710</v>
+      </c>
+      <c r="B1583" t="n">
+        <v>1184</v>
+      </c>
+      <c r="C1583" t="n">
+        <v>12119</v>
+      </c>
+      <c r="D1583" t="n">
+        <v>9.769782985394833</v>
+      </c>
+      <c r="E1583" t="n">
+        <v>740000</v>
+      </c>
+      <c r="F1583" t="b">
+        <v>0</v>
+      </c>
+      <c r="G1583" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>